<commit_message>
Some more changes to streamline code
</commit_message>
<xml_diff>
--- a/Scripts_AGORA2_Heinken_et_al_2022/input/knownDrugMetabolizers.xlsx
+++ b/Scripts_AGORA2_Heinken_et_al_2022/input/knownDrugMetabolizers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AGORA2_rerunEverything\Scripts\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AGORA2_rerunEverything\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D634FDC1-8ED2-4578-ADEB-F66C1533AB3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177AEDDE-1C50-43F2-8AE5-577DE11FBE7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="645" windowWidth="24945" windowHeight="14025" xr2:uid="{5F7D4F41-A766-3542-89FB-D98ABF6951FC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5F7D4F41-A766-3542-89FB-D98ABF6951FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Table_Sx2" sheetId="1" r:id="rId1"/>
@@ -155,9 +155,6 @@
     <t>Bacteroides_uniformis_ATCC_8492</t>
   </si>
   <si>
-    <t>Bacteroides_vulgatus</t>
-  </si>
-  <si>
     <t>Bifidobacterium_adolescentis_ATCC_15703</t>
   </si>
   <si>
@@ -554,9 +551,6 @@
     <t>VMH ID of corresponding reaction(s)</t>
   </si>
   <si>
-    <t>BZD_AR_NAD,BZD_AR_NADP</t>
-  </si>
-  <si>
     <t>5-fluorocytosine via cytosine deaminase</t>
   </si>
   <si>
@@ -692,9 +686,6 @@
     <t>PMID:15870453</t>
   </si>
   <si>
-    <t>Clostridium_innocuum</t>
-  </si>
-  <si>
     <t>Paraeggerthella_hongkongensis_RC2_2</t>
   </si>
   <si>
@@ -710,9 +701,6 @@
     <t>Methanosphaera_stadtmanae</t>
   </si>
   <si>
-    <t>Lachnoclostridium_clostridioforme</t>
-  </si>
-  <si>
     <t>Levilactobacillus_brevis</t>
   </si>
   <si>
@@ -726,6 +714,18 @@
   </si>
   <si>
     <t>Limosilactobacillus_fermentum</t>
+  </si>
+  <si>
+    <t>BZD_AR_NADi,BZD_AR_NADPi</t>
+  </si>
+  <si>
+    <t>Phocaeicola_vulgatus</t>
+  </si>
+  <si>
+    <t>Enterocloster_clostridioformis</t>
+  </si>
+  <si>
+    <t>Erysipelatoclostridium_innocuum</t>
   </si>
 </sst>
 </file>
@@ -1119,15 +1119,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB201F79-648D-3149-B3D0-550C48F7934C}">
   <dimension ref="A1:U254"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A234" workbookViewId="0">
-      <selection activeCell="A243" sqref="A243"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41" style="3" customWidth="1"/>
     <col min="2" max="2" width="16.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="43" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="20" style="1" customWidth="1"/>
@@ -1151,19 +1151,19 @@
         <v>19</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>2</v>
@@ -1188,10 +1188,10 @@
         <v>30</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>1</v>
@@ -1207,10 +1207,10 @@
         <v>27</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>1</v>
@@ -1226,10 +1226,10 @@
         <v>28</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>1</v>
@@ -1242,13 +1242,13 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>0</v>
@@ -1261,13 +1261,13 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>0</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>0</v>
@@ -1299,13 +1299,13 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>1</v>
@@ -1318,13 +1318,13 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>1</v>
@@ -1338,13 +1338,13 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>0</v>
@@ -1357,13 +1357,13 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C11" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>1</v>
@@ -1376,13 +1376,13 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>1</v>
@@ -1396,13 +1396,13 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C13" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>1</v>
@@ -1415,13 +1415,13 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>0</v>
@@ -1434,13 +1434,13 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C15" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>1</v>
@@ -1453,13 +1453,13 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C16" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>1</v>
@@ -1472,13 +1472,13 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C17" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>1</v>
@@ -1491,13 +1491,13 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C18" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>1</v>
@@ -1510,13 +1510,13 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C19" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>1</v>
@@ -1529,13 +1529,13 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C20" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>1</v>
@@ -1548,13 +1548,13 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C21" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>1</v>
@@ -1567,13 +1567,13 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C22" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>1</v>
@@ -1586,13 +1586,13 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C23" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>0</v>
@@ -1606,13 +1606,13 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C24" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>0</v>
@@ -1625,13 +1625,13 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C25" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>1</v>
@@ -1655,13 +1655,13 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C26" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>1</v>
@@ -1674,13 +1674,13 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C27" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>1</v>
@@ -1693,13 +1693,13 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C28" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>1</v>
@@ -1712,13 +1712,13 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C29" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>1</v>
@@ -1731,13 +1731,13 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C30" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>1</v>
@@ -1750,13 +1750,13 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C31" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>1</v>
@@ -1769,13 +1769,13 @@
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C32" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>0</v>
@@ -1783,18 +1783,18 @@
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
       <c r="G32" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C33" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>0</v>
@@ -1821,10 +1821,10 @@
         <v>31</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C34" t="s">
-        <v>173</v>
+        <v>227</v>
       </c>
       <c r="D34" s="8" t="s">
         <v>0</v>
@@ -1832,18 +1832,18 @@
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C35" t="s">
-        <v>173</v>
+        <v>227</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>0</v>
@@ -1851,7 +1851,7 @@
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
       <c r="G35" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
@@ -1859,10 +1859,10 @@
         <v>38</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C36" t="s">
-        <v>173</v>
+        <v>227</v>
       </c>
       <c r="D36" s="8" t="s">
         <v>1</v>
@@ -1875,13 +1875,13 @@
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C37" t="s">
-        <v>173</v>
+        <v>227</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>1</v>
@@ -1894,13 +1894,13 @@
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C38" t="s">
-        <v>173</v>
+        <v>227</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>1</v>
@@ -1928,10 +1928,10 @@
         <v>39</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C39" t="s">
-        <v>173</v>
+        <v>227</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>0</v>
@@ -1944,13 +1944,13 @@
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C40" t="s">
-        <v>173</v>
+        <v>227</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>0</v>
@@ -1963,13 +1963,13 @@
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C41" t="s">
-        <v>173</v>
+        <v>227</v>
       </c>
       <c r="D41" s="8" t="s">
         <v>1</v>
@@ -1982,13 +1982,13 @@
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C42" t="s">
-        <v>173</v>
+        <v>227</v>
       </c>
       <c r="D42" s="8" t="s">
         <v>1</v>
@@ -2001,13 +2001,13 @@
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C43" t="s">
-        <v>173</v>
+        <v>227</v>
       </c>
       <c r="D43" s="8" t="s">
         <v>1</v>
@@ -2020,13 +2020,13 @@
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C44" t="s">
-        <v>173</v>
+        <v>227</v>
       </c>
       <c r="D44" s="8" t="s">
         <v>0</v>
@@ -2039,13 +2039,13 @@
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C45" t="s">
-        <v>173</v>
+        <v>227</v>
       </c>
       <c r="D45" s="8" t="s">
         <v>0</v>
@@ -2058,13 +2058,13 @@
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C46" t="s">
-        <v>173</v>
+        <v>227</v>
       </c>
       <c r="D46" s="8" t="s">
         <v>0</v>
@@ -2077,13 +2077,13 @@
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C47" t="s">
-        <v>173</v>
+        <v>227</v>
       </c>
       <c r="D47" s="8" t="s">
         <v>0</v>
@@ -2096,13 +2096,13 @@
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C48" t="s">
-        <v>173</v>
+        <v>227</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>0</v>
@@ -2110,19 +2110,19 @@
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
       <c r="G48" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="S48"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C49" t="s">
-        <v>173</v>
+        <v>227</v>
       </c>
       <c r="D49" s="8" t="s">
         <v>0</v>
@@ -2135,13 +2135,13 @@
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C50" t="s">
-        <v>173</v>
+        <v>227</v>
       </c>
       <c r="D50" s="8" t="s">
         <v>0</v>
@@ -2149,19 +2149,19 @@
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
       <c r="G50" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="S50"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C51" t="s">
-        <v>173</v>
+        <v>227</v>
       </c>
       <c r="D51" s="8" t="s">
         <v>0</v>
@@ -2169,18 +2169,18 @@
       <c r="E51" s="8"/>
       <c r="F51" s="8"/>
       <c r="G51" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C52" t="s">
-        <v>173</v>
+        <v>227</v>
       </c>
       <c r="D52" s="8" t="s">
         <v>0</v>
@@ -2188,18 +2188,18 @@
       <c r="E52" s="8"/>
       <c r="F52" s="8"/>
       <c r="G52" s="8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C53" t="s">
-        <v>173</v>
+        <v>227</v>
       </c>
       <c r="D53" s="8" t="s">
         <v>0</v>
@@ -2207,19 +2207,19 @@
       <c r="E53" s="8"/>
       <c r="F53" s="8"/>
       <c r="G53" s="8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="S53"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C54" t="s">
-        <v>173</v>
+        <v>227</v>
       </c>
       <c r="D54" s="8" t="s">
         <v>0</v>
@@ -2227,18 +2227,18 @@
       <c r="E54" s="8"/>
       <c r="F54" s="8"/>
       <c r="G54" s="8" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C55" t="s">
-        <v>173</v>
+        <v>227</v>
       </c>
       <c r="D55" s="8" t="s">
         <v>0</v>
@@ -2246,7 +2246,7 @@
       <c r="E55" s="8"/>
       <c r="F55" s="8"/>
       <c r="G55" s="8" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
@@ -2254,10 +2254,10 @@
         <v>38</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C56" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D56" s="8" t="s">
         <v>0</v>
@@ -2270,13 +2270,13 @@
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C57" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D57" s="8" t="s">
         <v>0</v>
@@ -2289,13 +2289,13 @@
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C58" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D58" s="8" t="s">
         <v>0</v>
@@ -2311,10 +2311,10 @@
         <v>39</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C59" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D59" s="8" t="s">
         <v>0</v>
@@ -2327,13 +2327,13 @@
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C60" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D60" s="8" t="s">
         <v>0</v>
@@ -2346,13 +2346,13 @@
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C61" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D61" s="8" t="s">
         <v>0</v>
@@ -2365,13 +2365,13 @@
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C62" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D62" s="8" t="s">
         <v>0</v>
@@ -2384,13 +2384,13 @@
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C63" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D63" s="8" t="s">
         <v>0</v>
@@ -2415,13 +2415,13 @@
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C64" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D64" s="8" t="s">
         <v>0</v>
@@ -2446,13 +2446,13 @@
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C65" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D65" s="8" t="s">
         <v>0</v>
@@ -2465,13 +2465,13 @@
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C66" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D66" s="8" t="s">
         <v>0</v>
@@ -2485,13 +2485,13 @@
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C67" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D67" s="8" t="s">
         <v>0</v>
@@ -2505,13 +2505,13 @@
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C68" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D68" s="8" t="s">
         <v>0</v>
@@ -2525,13 +2525,13 @@
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C69" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D69" s="8" t="s">
         <v>0</v>
@@ -2544,13 +2544,13 @@
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C70" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D70" s="8" t="s">
         <v>0</v>
@@ -2569,7 +2569,7 @@
         <v>24</v>
       </c>
       <c r="C71" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D71" s="8" t="s">
         <v>1</v>
@@ -2588,7 +2588,7 @@
         <v>24</v>
       </c>
       <c r="C72" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D72" s="8" t="s">
         <v>0</v>
@@ -2608,7 +2608,7 @@
         <v>24</v>
       </c>
       <c r="C73" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D73" s="8" t="s">
         <v>0</v>
@@ -2621,13 +2621,13 @@
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B74" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C74" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D74" s="8" t="s">
         <v>1</v>
@@ -2640,13 +2640,13 @@
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B75" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C75" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D75" s="8" t="s">
         <v>1</v>
@@ -2659,13 +2659,13 @@
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B76" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C76" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D76" s="8" t="s">
         <v>1</v>
@@ -2678,13 +2678,13 @@
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B77" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C77" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D77" s="8" t="s">
         <v>0</v>
@@ -2697,13 +2697,13 @@
     </row>
     <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B78" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C78" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D78" s="8" t="s">
         <v>1</v>
@@ -2716,13 +2716,13 @@
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B79" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C79" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D79" s="8" t="s">
         <v>0</v>
@@ -2735,13 +2735,13 @@
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B80" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C80" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D80" s="8" t="s">
         <v>0</v>
@@ -2754,13 +2754,13 @@
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A81" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B81" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C81" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D81" s="8" t="s">
         <v>1</v>
@@ -2773,13 +2773,13 @@
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B82" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C82" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D82" s="8" t="s">
         <v>1</v>
@@ -2792,13 +2792,13 @@
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B83" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C83" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D83" s="8" t="s">
         <v>1</v>
@@ -2811,13 +2811,13 @@
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B84" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C84" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D84" s="8" t="s">
         <v>0</v>
@@ -2830,13 +2830,13 @@
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B85" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C85" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D85" s="8" t="s">
         <v>1</v>
@@ -2849,13 +2849,13 @@
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B86" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C86" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D86" s="8" t="s">
         <v>1</v>
@@ -2868,13 +2868,13 @@
     </row>
     <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B87" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C87" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D87" s="8" t="s">
         <v>1</v>
@@ -2893,7 +2893,7 @@
         <v>8</v>
       </c>
       <c r="C88" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D88" s="8" t="s">
         <v>1</v>
@@ -2906,13 +2906,13 @@
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B89" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C89" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D89" s="8" t="s">
         <v>1</v>
@@ -2925,13 +2925,13 @@
     </row>
     <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B90" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C90" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D90" s="8" t="s">
         <v>1</v>
@@ -2944,13 +2944,13 @@
     </row>
     <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A91" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B91" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C91" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D91" s="8" t="s">
         <v>1</v>
@@ -2963,13 +2963,13 @@
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A92" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B92" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C92" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D92" s="8" t="s">
         <v>1</v>
@@ -2983,13 +2983,13 @@
     </row>
     <row r="93" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B93" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C93" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D93" s="8" t="s">
         <v>1</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="94" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A94" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B94" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C94" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D94" s="8" t="s">
         <v>1</v>
@@ -3021,13 +3021,13 @@
     </row>
     <row r="95" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A95" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B95" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C95" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D95" s="8" t="s">
         <v>1</v>
@@ -3040,13 +3040,13 @@
     </row>
     <row r="96" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A96" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B96" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C96" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D96" s="8" t="s">
         <v>1</v>
@@ -3059,13 +3059,13 @@
     </row>
     <row r="97" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A97" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B97" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C97" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D97" s="8" t="s">
         <v>1</v>
@@ -3078,13 +3078,13 @@
     </row>
     <row r="98" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A98" s="8" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B98" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C98" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D98" s="8" t="s">
         <v>1</v>
@@ -3097,13 +3097,13 @@
     </row>
     <row r="99" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A99" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B99" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C99" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D99" s="8" t="s">
         <v>1</v>
@@ -3116,13 +3116,13 @@
     </row>
     <row r="100" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A100" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B100" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C100" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D100" s="8" t="s">
         <v>1</v>
@@ -3135,13 +3135,13 @@
     </row>
     <row r="101" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B101" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C101" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D101" s="8" t="s">
         <v>1</v>
@@ -3154,13 +3154,13 @@
     </row>
     <row r="102" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A102" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B102" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C102" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D102" s="8" t="s">
         <v>1</v>
@@ -3173,13 +3173,13 @@
     </row>
     <row r="103" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A103" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B103" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C103" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D103" s="8" t="s">
         <v>1</v>
@@ -3192,13 +3192,13 @@
     </row>
     <row r="104" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A104" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B104" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C104" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D104" s="8" t="s">
         <v>1</v>
@@ -3211,13 +3211,13 @@
     </row>
     <row r="105" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A105" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B105" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C105" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D105" s="8" t="s">
         <v>1</v>
@@ -3230,13 +3230,13 @@
     </row>
     <row r="106" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A106" s="8" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B106" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C106" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D106" s="8" t="s">
         <v>1</v>
@@ -3249,13 +3249,13 @@
     </row>
     <row r="107" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A107" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C107" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D107" s="8" t="s">
         <v>1</v>
@@ -3263,18 +3263,18 @@
       <c r="E107" s="8"/>
       <c r="F107" s="8"/>
       <c r="G107" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="108" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A108" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C108" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D108" s="8" t="s">
         <v>1</v>
@@ -3282,18 +3282,18 @@
       <c r="E108" s="8"/>
       <c r="F108" s="8"/>
       <c r="G108" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="109" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A109" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C109" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D109" s="8" t="s">
         <v>1</v>
@@ -3301,18 +3301,18 @@
       <c r="E109" s="8"/>
       <c r="F109" s="8"/>
       <c r="G109" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="110" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A110" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C110" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D110" s="8" t="s">
         <v>0</v>
@@ -3320,18 +3320,18 @@
       <c r="E110" s="8"/>
       <c r="F110" s="8"/>
       <c r="G110" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="111" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A111" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C111" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D111" s="8" t="s">
         <v>0</v>
@@ -3339,7 +3339,7 @@
       <c r="E111" s="8"/>
       <c r="F111" s="8"/>
       <c r="G111" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I111"/>
       <c r="J111"/>
@@ -3355,13 +3355,13 @@
     </row>
     <row r="112" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A112" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C112" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D112" s="8" t="s">
         <v>0</v>
@@ -3369,18 +3369,18 @@
       <c r="E112" s="8"/>
       <c r="F112" s="8"/>
       <c r="G112" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="113" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A113" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C113" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D113" s="8" t="s">
         <v>1</v>
@@ -3388,7 +3388,7 @@
       <c r="E113" s="8"/>
       <c r="F113" s="8"/>
       <c r="G113" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I113"/>
       <c r="J113"/>
@@ -3404,13 +3404,13 @@
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A114" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C114" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D114" s="8" t="s">
         <v>0</v>
@@ -3418,18 +3418,18 @@
       <c r="E114" s="8"/>
       <c r="F114" s="8"/>
       <c r="G114" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="115" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A115" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C115" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D115" s="8" t="s">
         <v>0</v>
@@ -3437,18 +3437,18 @@
       <c r="E115" s="8"/>
       <c r="F115" s="8"/>
       <c r="G115" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="116" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A116" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C116" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D116" s="8" t="s">
         <v>0</v>
@@ -3456,18 +3456,18 @@
       <c r="E116" s="8"/>
       <c r="F116" s="8"/>
       <c r="G116" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="117" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A117" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C117" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D117" s="8" t="s">
         <v>0</v>
@@ -3475,7 +3475,7 @@
       <c r="E117" s="8"/>
       <c r="F117" s="8"/>
       <c r="G117" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I117"/>
       <c r="J117"/>
@@ -3491,13 +3491,13 @@
     </row>
     <row r="118" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A118" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C118" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D118" s="8" t="s">
         <v>1</v>
@@ -3505,18 +3505,18 @@
       <c r="E118" s="8"/>
       <c r="F118" s="8"/>
       <c r="G118" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="119" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A119" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C119" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D119" s="8" t="s">
         <v>1</v>
@@ -3524,18 +3524,18 @@
       <c r="E119" s="8"/>
       <c r="F119" s="8"/>
       <c r="G119" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="120" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A120" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C120" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D120" s="8" t="s">
         <v>1</v>
@@ -3543,7 +3543,7 @@
       <c r="E120" s="8"/>
       <c r="F120" s="8"/>
       <c r="G120" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I120"/>
       <c r="J120"/>
@@ -3559,13 +3559,13 @@
     </row>
     <row r="121" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A121" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C121" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D121" s="8" t="s">
         <v>0</v>
@@ -3573,18 +3573,18 @@
       <c r="E121" s="8"/>
       <c r="F121" s="8"/>
       <c r="G121" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="122" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A122" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C122" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D122" s="8" t="s">
         <v>0</v>
@@ -3592,18 +3592,18 @@
       <c r="E122" s="8"/>
       <c r="F122" s="8"/>
       <c r="G122" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="123" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A123" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C123" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D123" s="8" t="s">
         <v>0</v>
@@ -3611,18 +3611,18 @@
       <c r="E123" s="8"/>
       <c r="F123" s="8"/>
       <c r="G123" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="124" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A124" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C124" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D124" s="8" t="s">
         <v>0</v>
@@ -3630,7 +3630,7 @@
       <c r="E124" s="8"/>
       <c r="F124" s="8"/>
       <c r="G124" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I124"/>
       <c r="J124"/>
@@ -3646,13 +3646,13 @@
     </row>
     <row r="125" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A125" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C125" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D125" s="8" t="s">
         <v>1</v>
@@ -3660,7 +3660,7 @@
       <c r="E125" s="8"/>
       <c r="F125" s="8"/>
       <c r="G125" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I125"/>
       <c r="J125"/>
@@ -3676,13 +3676,13 @@
     </row>
     <row r="126" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A126" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C126" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D126" s="8" t="s">
         <v>1</v>
@@ -3690,18 +3690,18 @@
       <c r="E126" s="8"/>
       <c r="F126" s="8"/>
       <c r="G126" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="127" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A127" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C127" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D127" s="8" t="s">
         <v>1</v>
@@ -3709,7 +3709,7 @@
       <c r="E127" s="8"/>
       <c r="F127" s="8"/>
       <c r="G127" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="128" spans="1:19" x14ac:dyDescent="0.25">
@@ -3720,7 +3720,7 @@
         <v>7</v>
       </c>
       <c r="C128" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D128" s="8" t="s">
         <v>1</v>
@@ -3728,18 +3728,18 @@
       <c r="E128" s="8"/>
       <c r="F128" s="8"/>
       <c r="G128" s="8" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="129" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A129" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B129" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C129" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D129" s="8" t="s">
         <v>1</v>
@@ -3752,13 +3752,13 @@
     </row>
     <row r="130" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A130" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B130" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C130" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D130" s="8" t="s">
         <v>0</v>
@@ -3771,13 +3771,13 @@
     </row>
     <row r="131" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A131" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B131" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C131" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D131" s="8" t="s">
         <v>0</v>
@@ -3790,13 +3790,13 @@
     </row>
     <row r="132" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A132" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B132" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C132" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D132" s="8" t="s">
         <v>0</v>
@@ -3809,13 +3809,13 @@
     </row>
     <row r="133" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A133" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B133" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C133" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D133" s="8" t="s">
         <v>0</v>
@@ -3828,13 +3828,13 @@
     </row>
     <row r="134" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A134" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B134" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C134" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D134" s="8" t="s">
         <v>0</v>
@@ -3848,13 +3848,13 @@
     </row>
     <row r="135" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A135" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B135" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C135" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D135" s="8" t="s">
         <v>0</v>
@@ -3867,13 +3867,13 @@
     </row>
     <row r="136" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A136" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B136" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C136" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D136" s="8" t="s">
         <v>0</v>
@@ -3886,13 +3886,13 @@
     </row>
     <row r="137" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A137" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B137" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C137" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D137" s="8" t="s">
         <v>1</v>
@@ -3900,18 +3900,18 @@
       <c r="E137" s="8"/>
       <c r="F137" s="8"/>
       <c r="G137" s="8" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="138" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A138" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B138" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C138" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D138" s="8" t="s">
         <v>1</v>
@@ -3919,18 +3919,18 @@
       <c r="E138" s="8"/>
       <c r="F138" s="8"/>
       <c r="G138" s="8" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="139" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A139" s="8" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B139" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C139" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D139" s="8" t="s">
         <v>0</v>
@@ -3938,18 +3938,18 @@
       <c r="E139" s="8"/>
       <c r="F139" s="8"/>
       <c r="G139" s="8" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="140" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A140" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B140" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C140" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D140" s="8" t="s">
         <v>1</v>
@@ -3957,18 +3957,18 @@
       <c r="E140" s="8"/>
       <c r="F140" s="8"/>
       <c r="G140" s="8" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="141" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A141" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B141" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C141" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D141" s="8" t="s">
         <v>1</v>
@@ -3981,13 +3981,13 @@
     </row>
     <row r="142" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A142" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B142" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C142" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D142" s="8" t="s">
         <v>0</v>
@@ -4001,13 +4001,13 @@
     </row>
     <row r="143" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A143" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B143" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C143" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D143" s="8" t="s">
         <v>0</v>
@@ -4015,18 +4015,18 @@
       <c r="E143" s="8"/>
       <c r="F143" s="8"/>
       <c r="G143" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="144" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A144" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B144" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C144" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D144" s="8" t="s">
         <v>0</v>
@@ -4034,18 +4034,18 @@
       <c r="E144" s="8"/>
       <c r="F144" s="8"/>
       <c r="G144" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B145" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C145" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D145" s="8" t="s">
         <v>0</v>
@@ -4053,18 +4053,18 @@
       <c r="E145" s="8"/>
       <c r="F145" s="8"/>
       <c r="G145" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B146" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C146" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D146" s="8" t="s">
         <v>1</v>
@@ -4072,18 +4072,18 @@
       <c r="E146" s="8"/>
       <c r="F146" s="8"/>
       <c r="G146" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B147" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C147" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D147" s="8" t="s">
         <v>1</v>
@@ -4091,18 +4091,18 @@
       <c r="E147" s="8"/>
       <c r="F147" s="8"/>
       <c r="G147" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B148" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C148" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D148" s="8" t="s">
         <v>0</v>
@@ -4110,18 +4110,18 @@
       <c r="E148" s="8"/>
       <c r="F148" s="8"/>
       <c r="G148" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B149" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C149" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D149" s="8" t="s">
         <v>0</v>
@@ -4129,18 +4129,18 @@
       <c r="E149" s="8"/>
       <c r="F149" s="8"/>
       <c r="G149" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B150" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C150" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D150" s="8" t="s">
         <v>1</v>
@@ -4148,18 +4148,18 @@
       <c r="E150" s="8"/>
       <c r="F150" s="8"/>
       <c r="G150" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B151" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C151" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D151" s="8" t="s">
         <v>0</v>
@@ -4167,18 +4167,18 @@
       <c r="E151" s="8"/>
       <c r="F151" s="8"/>
       <c r="G151" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="8" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B152" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C152" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D152" s="8" t="s">
         <v>0</v>
@@ -4186,18 +4186,18 @@
       <c r="E152" s="8"/>
       <c r="F152" s="8"/>
       <c r="G152" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B153" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C153" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D153" s="8" t="s">
         <v>0</v>
@@ -4205,18 +4205,18 @@
       <c r="E153" s="8"/>
       <c r="F153" s="8"/>
       <c r="G153" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B154" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C154" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D154" s="8" t="s">
         <v>0</v>
@@ -4224,18 +4224,18 @@
       <c r="E154" s="8"/>
       <c r="F154" s="8"/>
       <c r="G154" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B155" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C155" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D155" s="8" t="s">
         <v>0</v>
@@ -4243,18 +4243,18 @@
       <c r="E155" s="8"/>
       <c r="F155" s="8"/>
       <c r="G155" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B156" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C156" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D156" s="8" t="s">
         <v>0</v>
@@ -4262,18 +4262,18 @@
       <c r="E156" s="8"/>
       <c r="F156" s="8"/>
       <c r="G156" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B157" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C157" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D157" s="8" t="s">
         <v>0</v>
@@ -4281,18 +4281,18 @@
       <c r="E157" s="8"/>
       <c r="F157" s="8"/>
       <c r="G157" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B158" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C158" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D158" s="8" t="s">
         <v>1</v>
@@ -4300,18 +4300,18 @@
       <c r="E158" s="8"/>
       <c r="F158" s="8"/>
       <c r="G158" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B159" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C159" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D159" s="8" t="s">
         <v>0</v>
@@ -4319,18 +4319,18 @@
       <c r="E159" s="8"/>
       <c r="F159" s="8"/>
       <c r="G159" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B160" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C160" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D160" s="8" t="s">
         <v>1</v>
@@ -4338,18 +4338,18 @@
       <c r="E160" s="8"/>
       <c r="F160" s="8"/>
       <c r="G160" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="161" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A161" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B161" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C161" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D161" s="8" t="s">
         <v>0</v>
@@ -4357,18 +4357,18 @@
       <c r="E161" s="8"/>
       <c r="F161" s="8"/>
       <c r="G161" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="162" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A162" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B162" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C162" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D162" s="8" t="s">
         <v>0</v>
@@ -4376,18 +4376,18 @@
       <c r="E162" s="8"/>
       <c r="F162" s="8"/>
       <c r="G162" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="163" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A163" s="8" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B163" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C163" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D163" s="8" t="s">
         <v>0</v>
@@ -4395,18 +4395,18 @@
       <c r="E163" s="8"/>
       <c r="F163" s="8"/>
       <c r="G163" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="164" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A164" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B164" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C164" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D164" s="8" t="s">
         <v>0</v>
@@ -4414,18 +4414,18 @@
       <c r="E164" s="8"/>
       <c r="F164" s="8"/>
       <c r="G164" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="165" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A165" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B165" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C165" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D165" s="8" t="s">
         <v>0</v>
@@ -4433,18 +4433,18 @@
       <c r="E165" s="8"/>
       <c r="F165" s="8"/>
       <c r="G165" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="166" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A166" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B166" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C166" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D166" s="8" t="s">
         <v>0</v>
@@ -4452,18 +4452,18 @@
       <c r="E166" s="8"/>
       <c r="F166" s="8"/>
       <c r="G166" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="167" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A167" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B167" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C167" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D167" s="8" t="s">
         <v>0</v>
@@ -4471,18 +4471,18 @@
       <c r="E167" s="8"/>
       <c r="F167" s="8"/>
       <c r="G167" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="168" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A168" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B168" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C168" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D168" s="8" t="s">
         <v>0</v>
@@ -4490,18 +4490,18 @@
       <c r="E168" s="8"/>
       <c r="F168" s="8"/>
       <c r="G168" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="169" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A169" s="8" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B169" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C169" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D169" s="8" t="s">
         <v>0</v>
@@ -4509,18 +4509,18 @@
       <c r="E169" s="8"/>
       <c r="F169" s="8"/>
       <c r="G169" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="170" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A170" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B170" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C170" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D170" s="8" t="s">
         <v>0</v>
@@ -4528,18 +4528,18 @@
       <c r="E170" s="8"/>
       <c r="F170" s="8"/>
       <c r="G170" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="171" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A171" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B171" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C171" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D171" s="8" t="s">
         <v>0</v>
@@ -4547,18 +4547,18 @@
       <c r="E171" s="8"/>
       <c r="F171" s="8"/>
       <c r="G171" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="172" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A172" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B172" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C172" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D172" s="8" t="s">
         <v>0</v>
@@ -4566,19 +4566,19 @@
       <c r="E172" s="8"/>
       <c r="F172" s="8"/>
       <c r="G172" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="T172" s="1"/>
     </row>
     <row r="173" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A173" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B173" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C173" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D173" s="8" t="s">
         <v>0</v>
@@ -4586,18 +4586,18 @@
       <c r="E173" s="8"/>
       <c r="F173" s="8"/>
       <c r="G173" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="174" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A174" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B174" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C174" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D174" s="8" t="s">
         <v>0</v>
@@ -4605,18 +4605,18 @@
       <c r="E174" s="8"/>
       <c r="F174" s="8"/>
       <c r="G174" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="175" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A175" s="8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B175" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C175" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D175" s="8" t="s">
         <v>0</v>
@@ -4624,18 +4624,18 @@
       <c r="E175" s="8"/>
       <c r="F175" s="8"/>
       <c r="G175" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="176" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A176" s="8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B176" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C176" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D176" s="8" t="s">
         <v>0</v>
@@ -4643,18 +4643,18 @@
       <c r="E176" s="8"/>
       <c r="F176" s="8"/>
       <c r="G176" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="8" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B177" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C177" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D177" s="8" t="s">
         <v>0</v>
@@ -4662,18 +4662,18 @@
       <c r="E177" s="8"/>
       <c r="F177" s="8"/>
       <c r="G177" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B178" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C178" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D178" s="8" t="s">
         <v>0</v>
@@ -4681,18 +4681,18 @@
       <c r="E178" s="8"/>
       <c r="F178" s="8"/>
       <c r="G178" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B179" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C179" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D179" s="8" t="s">
         <v>1</v>
@@ -4700,18 +4700,18 @@
       <c r="E179" s="8"/>
       <c r="F179" s="8"/>
       <c r="G179" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B180" t="s">
         <v>20</v>
       </c>
       <c r="C180" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D180" t="s">
         <v>0</v>
@@ -4719,18 +4719,18 @@
       <c r="E180"/>
       <c r="F180"/>
       <c r="G180" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B181" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C181" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D181" s="8" t="s">
         <v>0</v>
@@ -4746,10 +4746,10 @@
         <v>38</v>
       </c>
       <c r="B182" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C182" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D182" s="8" t="s">
         <v>0</v>
@@ -4762,13 +4762,13 @@
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B183" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C183" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D183" s="8" t="s">
         <v>0</v>
@@ -4781,13 +4781,13 @@
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B184" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C184" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D184" s="8" t="s">
         <v>0</v>
@@ -4800,13 +4800,13 @@
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="8" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
       <c r="B185" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C185" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D185" s="8" t="s">
         <v>1</v>
@@ -4822,10 +4822,10 @@
         <v>39</v>
       </c>
       <c r="B186" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C186" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D186" s="8" t="s">
         <v>0</v>
@@ -4838,13 +4838,13 @@
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B187" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C187" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D187" s="8" t="s">
         <v>0</v>
@@ -4857,13 +4857,13 @@
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B188" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C188" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D188" s="8" t="s">
         <v>0</v>
@@ -4876,13 +4876,13 @@
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B189" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C189" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D189" s="8" t="s">
         <v>1</v>
@@ -4895,13 +4895,13 @@
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B190" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C190" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D190" s="8" t="s">
         <v>0</v>
@@ -4914,13 +4914,13 @@
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="8" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B191" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C191" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D191" s="8" t="s">
         <v>0</v>
@@ -4933,13 +4933,13 @@
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B192" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C192" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D192" s="8" t="s">
         <v>0</v>
@@ -4952,13 +4952,13 @@
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B193" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C193" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D193" s="8" t="s">
         <v>0</v>
@@ -4971,13 +4971,13 @@
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B194" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C194" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D194" s="8" t="s">
         <v>0</v>
@@ -4990,13 +4990,13 @@
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B195" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C195" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D195" s="8" t="s">
         <v>0</v>
@@ -5009,13 +5009,13 @@
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B196" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C196" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D196" s="8" t="s">
         <v>0</v>
@@ -5023,18 +5023,18 @@
       <c r="E196" s="8"/>
       <c r="F196" s="8"/>
       <c r="G196" s="8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B197" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C197" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D197" s="8" t="s">
         <v>0</v>
@@ -5047,13 +5047,13 @@
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B198" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C198" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D198" s="8" t="s">
         <v>0</v>
@@ -5066,13 +5066,13 @@
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" s="8" t="s">
-        <v>40</v>
+        <v>228</v>
       </c>
       <c r="B199" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C199" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D199" s="8" t="s">
         <v>0</v>
@@ -5085,13 +5085,13 @@
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B200" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C200" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D200" s="8" t="s">
         <v>0</v>
@@ -5104,13 +5104,13 @@
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B201" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C201" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D201" s="8" t="s">
         <v>0</v>
@@ -5123,13 +5123,13 @@
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B202" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C202" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D202" s="8" t="s">
         <v>0</v>
@@ -5148,7 +5148,7 @@
         <v>10</v>
       </c>
       <c r="C203" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D203" s="8" t="s">
         <v>1</v>
@@ -5167,7 +5167,7 @@
         <v>10</v>
       </c>
       <c r="C204" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D204" s="8" t="s">
         <v>1</v>
@@ -5186,7 +5186,7 @@
         <v>10</v>
       </c>
       <c r="C205" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D205" s="8" t="s">
         <v>0</v>
@@ -5205,7 +5205,7 @@
         <v>10</v>
       </c>
       <c r="C206" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D206" s="8" t="s">
         <v>0</v>
@@ -5224,7 +5224,7 @@
         <v>10</v>
       </c>
       <c r="C207" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D207" s="8" t="s">
         <v>0</v>
@@ -5243,7 +5243,7 @@
         <v>10</v>
       </c>
       <c r="C208" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D208" s="8" t="s">
         <v>0</v>
@@ -5256,13 +5256,13 @@
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" s="8" t="s">
-        <v>40</v>
+        <v>228</v>
       </c>
       <c r="B209" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C209" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D209" s="8" t="s">
         <v>0</v>
@@ -5275,13 +5275,13 @@
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B210" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C210" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D210" s="8" t="s">
         <v>1</v>
@@ -5294,13 +5294,13 @@
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B211" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C211" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D211" s="8" t="s">
         <v>1</v>
@@ -5313,13 +5313,13 @@
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A212" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B212" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C212" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D212" s="8" t="s">
         <v>1</v>
@@ -5332,13 +5332,13 @@
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B213" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C213" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D213" s="8" t="s">
         <v>1</v>
@@ -5351,13 +5351,13 @@
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B214" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C214" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D214" s="8" t="s">
         <v>0</v>
@@ -5370,13 +5370,13 @@
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B215" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C215" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D215" s="8" t="s">
         <v>0</v>
@@ -5389,13 +5389,13 @@
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B216" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C216" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D216" s="8" t="s">
         <v>1</v>
@@ -5408,13 +5408,13 @@
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B217" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C217" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D217" s="8" t="s">
         <v>1</v>
@@ -5427,13 +5427,13 @@
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B218" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C218" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D218" s="8" t="s">
         <v>1</v>
@@ -5446,13 +5446,13 @@
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B219" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C219" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D219" s="8" t="s">
         <v>1</v>
@@ -5465,13 +5465,13 @@
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B220" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C220" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D220" s="8" t="s">
         <v>1</v>
@@ -5484,13 +5484,13 @@
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221" s="8" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B221" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C221" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D221" s="8" t="s">
         <v>1</v>
@@ -5503,13 +5503,13 @@
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222" s="8" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B222" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C222" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D222" s="8" t="s">
         <v>1</v>
@@ -5528,7 +5528,7 @@
         <v>10</v>
       </c>
       <c r="C223" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D223" s="8" t="s">
         <v>1</v>
@@ -5541,13 +5541,13 @@
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224" s="8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B224" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C224" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D224" s="8" t="s">
         <v>1</v>
@@ -5560,13 +5560,13 @@
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B225" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C225" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D225" s="8" t="s">
         <v>1</v>
@@ -5579,13 +5579,13 @@
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B226" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C226" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D226" s="8" t="s">
         <v>1</v>
@@ -5598,13 +5598,13 @@
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" s="8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B227" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C227" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D227" s="8" t="s">
         <v>1</v>
@@ -5617,13 +5617,13 @@
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B228" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C228" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D228" s="8" t="s">
         <v>1</v>
@@ -5636,13 +5636,13 @@
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B229" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C229" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D229" s="8" t="s">
         <v>1</v>
@@ -5655,13 +5655,13 @@
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230" s="8" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B230" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C230" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D230" s="8" t="s">
         <v>1</v>
@@ -5674,13 +5674,13 @@
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B231" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C231" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D231" s="8" t="s">
         <v>1</v>
@@ -5696,10 +5696,10 @@
         <v>35</v>
       </c>
       <c r="B232" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C232" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D232" s="8" t="s">
         <v>0</v>
@@ -5707,18 +5707,18 @@
       <c r="E232" s="8"/>
       <c r="F232" s="8"/>
       <c r="G232" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B233" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C233" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D233" s="8" t="s">
         <v>0</v>
@@ -5726,18 +5726,18 @@
       <c r="E233" s="8"/>
       <c r="F233" s="8"/>
       <c r="G233" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B234" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C234" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D234" s="8" t="s">
         <v>0</v>
@@ -5745,18 +5745,18 @@
       <c r="E234" s="8"/>
       <c r="F234" s="8"/>
       <c r="G234" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A235" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B235" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C235" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D235" s="8" t="s">
         <v>0</v>
@@ -5764,18 +5764,18 @@
       <c r="E235" s="8"/>
       <c r="F235" s="8"/>
       <c r="G235" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B236" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C236" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D236" s="8" t="s">
         <v>0</v>
@@ -5783,18 +5783,18 @@
       <c r="E236" s="8"/>
       <c r="F236" s="8"/>
       <c r="G236" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B237" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C237" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D237" s="8" t="s">
         <v>0</v>
@@ -5802,18 +5802,18 @@
       <c r="E237" s="8"/>
       <c r="F237" s="8"/>
       <c r="G237" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B238" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C238" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D238" s="8" t="s">
         <v>0</v>
@@ -5821,18 +5821,18 @@
       <c r="E238" s="8"/>
       <c r="F238" s="8"/>
       <c r="G238" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B239" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C239" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D239" s="8" t="s">
         <v>0</v>
@@ -5840,18 +5840,18 @@
       <c r="E239" s="8"/>
       <c r="F239" s="8"/>
       <c r="G239" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B240" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C240" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D240" s="8" t="s">
         <v>0</v>
@@ -5859,18 +5859,18 @@
       <c r="E240" s="8"/>
       <c r="F240" s="8"/>
       <c r="G240" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B241" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C241" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D241" s="8" t="s">
         <v>0</v>
@@ -5878,18 +5878,18 @@
       <c r="E241" s="8"/>
       <c r="F241" s="8"/>
       <c r="G241" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A242" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B242" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C242" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D242" s="8" t="s">
         <v>0</v>
@@ -5897,18 +5897,18 @@
       <c r="E242" s="8"/>
       <c r="F242" s="8"/>
       <c r="G242" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A243" s="8" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B243" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C243" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D243" s="8" t="s">
         <v>0</v>
@@ -5916,18 +5916,18 @@
       <c r="E243" s="8"/>
       <c r="F243" s="8"/>
       <c r="G243" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A244" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B244" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C244" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D244" s="8" t="s">
         <v>0</v>
@@ -5935,18 +5935,18 @@
       <c r="E244" s="8"/>
       <c r="F244" s="8"/>
       <c r="G244" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A245" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B245" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C245" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D245" s="8" t="s">
         <v>0</v>
@@ -5954,18 +5954,18 @@
       <c r="E245" s="8"/>
       <c r="F245" s="8"/>
       <c r="G245" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A246" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B246" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C246" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D246" s="8" t="s">
         <v>0</v>
@@ -5973,18 +5973,18 @@
       <c r="E246" s="8"/>
       <c r="F246" s="8"/>
       <c r="G246" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A247" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B247" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C247" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D247" s="8" t="s">
         <v>0</v>
@@ -5992,18 +5992,18 @@
       <c r="E247" s="8"/>
       <c r="F247" s="8"/>
       <c r="G247" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A248" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B248" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="B248" s="8" t="s">
-        <v>151</v>
-      </c>
       <c r="C248" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D248" s="8" t="s">
         <v>0</v>
@@ -6011,18 +6011,18 @@
       <c r="E248" s="8"/>
       <c r="F248" s="8"/>
       <c r="G248" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A249" s="8" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B249" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C249" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D249" s="8" t="s">
         <v>0</v>
@@ -6030,18 +6030,18 @@
       <c r="E249" s="8"/>
       <c r="F249" s="8"/>
       <c r="G249" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A250" s="8" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B250" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C250" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D250" s="8" t="s">
         <v>0</v>
@@ -6049,18 +6049,18 @@
       <c r="E250" s="8"/>
       <c r="F250" s="8"/>
       <c r="G250" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A251" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B251" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C251" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D251" s="8" t="s">
         <v>0</v>
@@ -6068,18 +6068,18 @@
       <c r="E251" s="8"/>
       <c r="F251" s="8"/>
       <c r="G251" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A252" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B252" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C252" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D252" s="8" t="s">
         <v>0</v>
@@ -6087,18 +6087,18 @@
       <c r="E252" s="8"/>
       <c r="F252" s="8"/>
       <c r="G252" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A253" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B253" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C253" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D253" s="8" t="s">
         <v>0</v>
@@ -6106,18 +6106,18 @@
       <c r="E253" s="8"/>
       <c r="F253" s="8"/>
       <c r="G253" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A254" s="8" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B254" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C254" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D254" s="8" t="s">
         <v>0</v>
@@ -6125,7 +6125,7 @@
       <c r="E254" s="8"/>
       <c r="F254" s="8"/>
       <c r="G254" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -6400,7 +6400,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB1499C-78A6-4926-8273-D68F59D1CE14}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CBD8EE5-99CB-4112-B782-4FB587E99BFE}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>